<commit_message>
normalized texts, streamlit structure
</commit_message>
<xml_diff>
--- a/data/processed/classify_data_htr_transcrip.xlsx
+++ b/data/processed/classify_data_htr_transcrip.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,82 +461,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>local_type_scheme</t>
+          <t>type_count</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>local_type</t>
+          <t>collection</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>mapping_status</t>
+          <t>volume_no</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>mapping_relation</t>
+          <t>source_ref</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>gold_status</t>
+          <t>atu_labels_json</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>type_count</t>
+          <t>txt_path</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>atu_labels_json</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>txt_path</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
           <t>text_raw</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>collection</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>volume_no</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>source_ref</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>type_code_1</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>type_code_2</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>type_code_3</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>type_code_4</t>
         </is>
       </c>
     </row>
@@ -566,37 +521,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 1, 503/4 (1)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>3</v>
+          <t>["402"]</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_1_503_1.txt</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
-        <is>
-          <t>["402"]</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_1_503_1.txt</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
         <is>
           <t xml:space="preserve">Тили были царь с царицей у не
 было три сына. Царица померла «яну
@@ -631,13 +582,6 @@
 </t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -666,45 +610,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>EE</t>
-        </is>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>424*</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 1, 515/6 (1)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
+          <t>["410"]</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_1_515_1.txt</t>
+        </is>
       </c>
       <c r="L3" t="inlineStr">
-        <is>
-          <t>["410"]</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_1_515_1.txt</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
         <is>
           <t xml:space="preserve">Раз пяное, ребятище» подился.
 что можит в 12 часов ночи принесо
@@ -743,13 +675,6 @@
 </t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -777,37 +702,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>12</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 105 (22)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>3</v>
+          <t>["703*"]</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_105_22.txt</t>
+        </is>
       </c>
       <c r="L4" t="inlineStr">
-        <is>
-          <t>["703*"]</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_105_22.txt</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
         <is>
           <t xml:space="preserve">Сделали дети со снегу куклу.
 В одного старина и старухи
@@ -824,13 +745,6 @@
 </t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -858,37 +772,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>12</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 137/41 (98)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>4</v>
+          <t>["530"]</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_137_98.txt</t>
+        </is>
       </c>
       <c r="L5" t="inlineStr">
-        <is>
-          <t>["530"]</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_137_98.txt</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
         <is>
           <t xml:space="preserve">Кил-был стажк. В яво бло
 тра сегна. Миша, Гриша и
@@ -984,13 +894,6 @@
 </t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1018,37 +921,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>12</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 189/94 (1)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>2</v>
+          <t>["735A"]</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_189_1.txt</t>
+        </is>
       </c>
       <c r="L6" t="inlineStr">
-        <is>
-          <t>["735A"]</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_189_1.txt</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
         <is>
           <t xml:space="preserve">Жили – брели два брата.
 и посла смерти отца оба
@@ -1154,13 +1053,6 @@
 </t>
         </is>
       </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1188,37 +1080,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>12</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 440/1 (19)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>3</v>
+          <t>["703*"]</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_440_19.txt</t>
+        </is>
       </c>
       <c r="L7" t="inlineStr">
-        <is>
-          <t>["703*"]</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_440_19.txt</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
         <is>
           <t xml:space="preserve">вили дед да бада и стали
 ен замой со снегу девочку
@@ -1236,13 +1124,6 @@
 </t>
         </is>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1270,45 +1151,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F8" t="n">
+        <v>5</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>480</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>12</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 12, 501/6 (1)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K8" t="n">
-        <v>5</v>
+          <t>["480D*"]</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_501_1.txt</t>
+        </is>
       </c>
       <c r="L8" t="inlineStr">
-        <is>
-          <t>["480D*"]</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_501_1.txt</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
         <is>
           <t xml:space="preserve">дрил мужем да баба Было
 в и двя дочери. Една было
@@ -1395,13 +1264,6 @@
 </t>
         </is>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1429,37 +1291,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 541/4 (1)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>2</v>
+          <t>["700"]</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_541_1.txt</t>
+        </is>
       </c>
       <c r="L9" t="inlineStr">
-        <is>
-          <t>["700"]</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_541_1.txt</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
         <is>
           <t xml:space="preserve">жбре старии да старуха,
 не брело в их дятей. Поехал
@@ -1542,13 +1400,6 @@
 </t>
         </is>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1576,37 +1427,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>12</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 592/4 (4)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>3</v>
+          <t>["703*"]</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_592_4.txt</t>
+        </is>
       </c>
       <c r="L10" t="inlineStr">
-        <is>
-          <t>["703*"]</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_592_4.txt</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
         <is>
           <t xml:space="preserve">Жия музик да баба стара
 люди были. Не брело в их дя
@@ -1651,13 +1498,6 @@
 </t>
         </is>
       </c>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1685,37 +1525,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>12</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 12, 95/7 (18)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K11" t="n">
-        <v>2</v>
+          <t>["700"]</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_95_18.txt</t>
+        </is>
       </c>
       <c r="L11" t="inlineStr">
-        <is>
-          <t>["700"]</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_95_18.txt</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
         <is>
           <t xml:space="preserve">бубил мужик дрова и отру¬
 был сей пальчила, брошл ен
@@ -1760,13 +1596,6 @@
 </t>
         </is>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1794,45 +1623,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F12" t="n">
+        <v>5</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>480</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>12</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 12, 97/101 (19)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K12" t="n">
-        <v>5</v>
+          <t>["480D*"]</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_97_19.txt</t>
+        </is>
       </c>
       <c r="L12" t="inlineStr">
-        <is>
-          <t>["480D*"]</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_12_97_19.txt</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
         <is>
           <t xml:space="preserve">Жили были дед да баба, не
 было в их дятей. Родилась де¬
@@ -1923,13 +1740,6 @@
 </t>
         </is>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1958,45 +1768,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>EE</t>
-        </is>
+      <c r="F13" t="n">
+        <v>3</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>424*</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>13</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 13, 106/24 (14)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K13" t="n">
-        <v>3</v>
+          <t>["307", "410"]</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_106_14.txt</t>
+        </is>
       </c>
       <c r="L13" t="inlineStr">
-        <is>
-          <t>["307", "410"]</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_106_14.txt</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
         <is>
           <t xml:space="preserve">14. В одной деревеньки жили два брата
 Листя и степан. Степон был че-
@@ -2375,13 +2173,6 @@
 </t>
         </is>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2410,45 +2201,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F14" t="n">
+        <v>3</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1060*</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>13</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 13, 137/50 (16)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>3</v>
+          <t>["650A", "1000", "1060"]</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_137_16.txt</t>
+        </is>
       </c>
       <c r="L14" t="inlineStr">
-        <is>
-          <t>["650A", "1000", "1060"]</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_137_16.txt</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
         <is>
           <t xml:space="preserve">16. Жин ной с попадьей. Брыло в
 н много земли, а раз зимли
@@ -2731,13 +2510,6 @@
 </t>
         </is>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2765,45 +2537,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F15" t="n">
+        <v>5</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>480</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 13, 15/9 (1)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>5</v>
+          <t>["480D*"]</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_15_1.txt</t>
+        </is>
       </c>
       <c r="L15" t="inlineStr">
-        <is>
-          <t>["480D*"]</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_15_1.txt</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr">
         <is>
           <t xml:space="preserve">1-2 Авдотья Ершова – 76 лет; деревья
 старый изборек. Всю жизнь прожила
@@ -2892,13 +2652,6 @@
 </t>
         </is>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2928,45 +2681,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F16" t="n">
+        <v>6</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>707B*</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>13</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 13, 175/202 (18)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K16" t="n">
-        <v>6</v>
+          <t>["707"]</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_175_18.txt</t>
+        </is>
       </c>
       <c r="L16" t="inlineStr">
-        <is>
-          <t>["707"]</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_175_18.txt</t>
-        </is>
-      </c>
-      <c r="N16" t="inlineStr">
         <is>
           <t xml:space="preserve">18. В некотором царстви втр
 десятом государстве иеня да был
@@ -3527,13 +3268,6 @@
 </t>
         </is>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3565,37 +3299,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>13</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 272/93 (23)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>1</v>
+          <t>["849*", "307"]</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_272_23.txt</t>
+        </is>
       </c>
       <c r="L17" t="inlineStr">
-        <is>
-          <t>["849*", "307"]</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_272_23.txt</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
         <is>
           <t xml:space="preserve">23. На горы, кун моря стояла
 ленька деревучка. Вси жихари этой
@@ -4025,13 +3755,6 @@
 </t>
         </is>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -4059,37 +3782,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F18" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>13</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 28/30 (3)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K18" t="n">
-        <v>3</v>
+          <t>["402"]</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_28_3.txt</t>
+        </is>
       </c>
       <c r="L18" t="inlineStr">
-        <is>
-          <t>["402"]</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_28_3.txt</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
         <is>
           <t xml:space="preserve">5. Жила злошшая баба, была
 в ей теронна дацка. В ктой
@@ -4143,13 +3862,6 @@
 </t>
         </is>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -4180,37 +3892,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>13</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 318/35 (27)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K19" t="n">
-        <v>4</v>
+          <t>["552", "580", "302С*", "556А*"]</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_318_27.txt</t>
+        </is>
       </c>
       <c r="L19" t="inlineStr">
-        <is>
-          <t>["552", "580", "302С*", "556А*"]</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_318_27.txt</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
         <is>
           <t xml:space="preserve">. Ватово Богатова еаря
 пали три дачки. Пошли ен
@@ -4570,13 +4278,6 @@
 </t>
         </is>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4604,37 +4305,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>13</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 37/42 (5)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K20" t="n">
-        <v>2</v>
+          <t>["706"]</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_37_5.txt</t>
+        </is>
       </c>
       <c r="L20" t="inlineStr">
-        <is>
-          <t>["706"]</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_37_5.txt</t>
-        </is>
-      </c>
-      <c r="N20" t="inlineStr">
         <is>
           <t xml:space="preserve">3. Перед смертью радители ско
 свому сыну: мы таперя
@@ -4764,13 +4461,6 @@
 </t>
         </is>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -4798,37 +4488,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>13</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 43/53 (6)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K21" t="n">
-        <v>3</v>
+          <t>["550"]</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_43_6.txt</t>
+        </is>
       </c>
       <c r="L21" t="inlineStr">
-        <is>
-          <t>["550"]</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_43_6.txt</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
         <is>
           <t xml:space="preserve">6. Шис царь. Было вниво три сына,
 извали не всие: Ваношками. Заболел
@@ -5039,13 +4725,6 @@
 </t>
         </is>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5073,37 +4752,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>13</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 635/8 (20)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K22" t="n">
-        <v>1</v>
+          <t>["470"]</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_635_20.txt</t>
+        </is>
       </c>
       <c r="L22" t="inlineStr">
-        <is>
-          <t>["470"]</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_635_20.txt</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
         <is>
           <t xml:space="preserve">30. Жили два мольца, дюжа
 оны сдруживши были.
@@ -5164,13 +4839,6 @@
 </t>
         </is>
       </c>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -5198,37 +4866,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>13</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 13, 73/9 (9)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K23" t="n">
-        <v>1</v>
+          <t>["511"]</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_73_9.txt</t>
+        </is>
       </c>
       <c r="L23" t="inlineStr">
-        <is>
-          <t>["511"]</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_13_73_9.txt</t>
-        </is>
-      </c>
-      <c r="N23" t="inlineStr">
         <is>
           <t xml:space="preserve">9. В некотором царстви, в тридесятом
 зарства пеше. мужин с бабой.
@@ -5364,13 +5028,6 @@
 </t>
         </is>
       </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -5398,45 +5055,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F24" t="n">
+        <v>3</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>650С*</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>14</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>close</t>
+          <t>ERA, Vene 14, 451 (7)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K24" t="n">
-        <v>3</v>
+          <t>["650A"]</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_14_451_7.txt</t>
+        </is>
       </c>
       <c r="L24" t="inlineStr">
-        <is>
-          <t>["650A"]</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_14_451_7.txt</t>
-        </is>
-      </c>
-      <c r="N24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 у. Салавей разбойник сидел на гр¬
@@ -5455,13 +5100,6 @@
 </t>
         </is>
       </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5489,37 +5127,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>15</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 15, 134/6 (3)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K25" t="n">
-        <v>3</v>
+          <t>["480A"]</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_134_3.txt</t>
+        </is>
       </c>
       <c r="L25" t="inlineStr">
-        <is>
-          <t>["480A"]</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_134_3.txt</t>
-        </is>
-      </c>
-      <c r="N25" t="inlineStr">
         <is>
           <t xml:space="preserve">Жил старик еа старухой
 и была у старухи свая дачка,
@@ -5571,13 +5205,6 @@
 </t>
         </is>
       </c>
-      <c r="O25" t="inlineStr"/>
-      <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -5606,37 +5233,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>15</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 15, 308/12 (4)</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K26" t="n">
-        <v>3</v>
+          <t>["480A"]</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_308_4.txt</t>
+        </is>
       </c>
       <c r="L26" t="inlineStr">
-        <is>
-          <t>["480A"]</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_308_4.txt</t>
-        </is>
-      </c>
-      <c r="N26" t="inlineStr">
         <is>
           <t xml:space="preserve">4. Жил дед еа старухой.
 них была двое дятей-бабника до
@@ -5709,13 +5332,6 @@
 </t>
         </is>
       </c>
-      <c r="O26" t="inlineStr"/>
-      <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5750,45 +5366,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F27" t="n">
+        <v>3</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>650В*</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>15</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>ERA, Vene 15, 433/52 (1)</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K27" t="n">
-        <v>3</v>
+          <t>["650A"]</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_433_1.txt</t>
+        </is>
       </c>
       <c r="L27" t="inlineStr">
-        <is>
-          <t>["650A"]</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_15_433_1.txt</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
         <is>
           <t xml:space="preserve">мыл царь Картау, а брат¬
 был Лазарь. У няво не была сына три¬
@@ -6165,13 +5769,6 @@
 </t>
         </is>
       </c>
-      <c r="O27" t="inlineStr"/>
-      <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -6199,37 +5796,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>16</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 16, 744 (22)</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K28" t="n">
-        <v>2</v>
+          <t>["300"]</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_16_744_22.txt</t>
+        </is>
       </c>
       <c r="L28" t="inlineStr">
-        <is>
-          <t>["300"]</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_16_744_22.txt</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
         <is>
           <t xml:space="preserve">. Тыл царь у няво была дочка.
 На берег выходит змен и каподый день
@@ -6247,13 +5840,6 @@
 </t>
         </is>
       </c>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -6281,37 +5867,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>16</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 16, 548/51 (4)</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K29" t="n">
-        <v>3</v>
+          <t>["402", "325"]</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_16_548_4.txt</t>
+        </is>
       </c>
       <c r="L29" t="inlineStr">
-        <is>
-          <t>["402", "325"]</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_16_548_4.txt</t>
-        </is>
-      </c>
-      <c r="N29" t="inlineStr">
         <is>
           <t xml:space="preserve">я. Шли маладые мальцы с
 монью и слышат что ва гу-
@@ -6371,13 +5953,6 @@
 </t>
         </is>
       </c>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -6405,37 +5980,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F30" t="n">
+        <v>6</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 2, 161/5 (14)</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K30" t="n">
-        <v>6</v>
+          <t>["707"]</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_161_14.txt</t>
+        </is>
       </c>
       <c r="L30" t="inlineStr">
-        <is>
-          <t>["707"]</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_161_14.txt</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Жил царь с царицей и был у них
@@ -6516,13 +6087,6 @@
 </t>
         </is>
       </c>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -6550,37 +6114,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 2, 622/6 (5)</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K31" t="n">
-        <v>2</v>
+          <t>["425C"]</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_622_5.txt</t>
+        </is>
       </c>
       <c r="L31" t="inlineStr">
-        <is>
-          <t>["425C"]</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_622_5.txt</t>
-        </is>
-      </c>
-      <c r="N31" t="inlineStr">
         <is>
           <t xml:space="preserve">Жил был на свете старин со ста¬
 рухой. У них было три дочки. Вот
@@ -6665,13 +6225,6 @@
 </t>
         </is>
       </c>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -6699,37 +6252,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 2, 748/9 (27)</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K32" t="n">
-        <v>3</v>
+          <t>["307"]</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_748_27.txt</t>
+        </is>
       </c>
       <c r="L32" t="inlineStr">
-        <is>
-          <t>["307"]</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_2_748_27.txt</t>
-        </is>
-      </c>
-      <c r="N32" t="inlineStr">
         <is>
           <t xml:space="preserve">Шли три человека, шли они
 лесом. Наступила ночь и
@@ -6766,13 +6315,6 @@
 </t>
         </is>
       </c>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -6804,37 +6346,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>4</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 4, 367/402 (1)</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K33" t="n">
-        <v>4</v>
+          <t>["530", "530A"]</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_4_367_1.txt</t>
+        </is>
       </c>
       <c r="L33" t="inlineStr">
-        <is>
-          <t>["530", "530A"]</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_4_367_1.txt</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
         <is>
           <t xml:space="preserve">ня лиднх да баба Былоя лизнака
 да бабы три сыпа, два у мыхда
@@ -7207,13 +6745,6 @@
 </t>
         </is>
       </c>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -7241,37 +6772,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F34" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>4</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 4, 403/29 (2)</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K34" t="n">
-        <v>6</v>
+          <t>["707"]</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_4_403_2.txt</t>
+        </is>
       </c>
       <c r="L34" t="inlineStr">
-        <is>
-          <t>["707"]</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_4_403_2.txt</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
         <is>
           <t xml:space="preserve">Ння был мужк и баба, было у них
 три девочки, но были они перодные,
@@ -7522,13 +7049,6 @@
 </t>
         </is>
       </c>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -7557,37 +7077,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>7</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 7, 95/9 (1)</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K35" t="n">
-        <v>2</v>
+          <t>["301"]</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_7_95_1.txt</t>
+        </is>
       </c>
       <c r="L35" t="inlineStr">
-        <is>
-          <t>["301"]</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_7_95_1.txt</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
         <is>
           <t xml:space="preserve">ил-был царь. В его зверинес
 30
@@ -7635,13 +7151,6 @@
 </t>
         </is>
       </c>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -7670,37 +7179,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>7</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 7, 71/2 (1)</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K36" t="n">
-        <v>2</v>
+          <t>["301"]</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_7_71_1.txt</t>
+        </is>
       </c>
       <c r="L36" t="inlineStr">
-        <is>
-          <t>["301"]</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_7_71_1.txt</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
         <is>
           <t xml:space="preserve">В некоторой цережые в некотором ансударстве; жил
 был царь! у этого жаря был сны Одивакды когда
@@ -7752,13 +7257,6 @@
 </t>
         </is>
       </c>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -7786,37 +7284,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>ERA, Vene</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>8</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>ERA, Vene 8, 210/1 (126)</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K37" t="n">
-        <v>3</v>
+          <t>["480A"]</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_8_210_126.txt</t>
+        </is>
       </c>
       <c r="L37" t="inlineStr">
-        <is>
-          <t>["480A"]</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/era_vene_8_210_126.txt</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
         <is>
           <t xml:space="preserve">Жыл дед и баба. У jих было две
 доцьке – у деда и у бабки. И баба
@@ -7854,13 +7348,6 @@
 </t>
         </is>
       </c>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
-      <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -7888,37 +7375,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>RKM, Vene</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>RKM, Vene 1, 236/44  (5)</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K38" t="n">
-        <v>1</v>
+          <t>["709"]</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/rkm_vene_1_236_5.txt</t>
+        </is>
       </c>
       <c r="L38" t="inlineStr">
-        <is>
-          <t>["709"]</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/rkm_vene_1_236_5.txt</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
         <is>
           <t xml:space="preserve">царь с царицей прастился,
 в путь зарогу нарязился, а
@@ -8092,13 +7575,6 @@
 </t>
         </is>
       </c>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -8128,37 +7604,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F39" t="n">
+        <v>6</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>RKM, Vene</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>RKM, Vene 1, 82/103 (47)</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K39" t="n">
-        <v>6</v>
+          <t>["707"]</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/rkm_vene_1_82_47.txt</t>
+        </is>
       </c>
       <c r="L39" t="inlineStr">
-        <is>
-          <t>["707"]</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/rkm_vene_1_82_47.txt</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
         <is>
           <t xml:space="preserve">в этаким, этаким царстве,
 в этаким, этаким государстве
@@ -8601,13 +8073,6 @@
 </t>
         </is>
       </c>
-      <c r="O39" t="inlineStr"/>
-      <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -8636,37 +8101,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F40" t="n">
+        <v>4</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>5</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 5, 36/43 (20)</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K40" t="n">
-        <v>4</v>
+          <t>["530"]</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_5_36_20.txt</t>
+        </is>
       </c>
       <c r="L40" t="inlineStr">
-        <is>
-          <t>["530"]</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_5_36_20.txt</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
         <is>
           <t xml:space="preserve">Жили -были у
 Были у них три сына; Два
@@ -8849,13 +8310,6 @@
 </t>
         </is>
       </c>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -8883,45 +8337,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F41" t="n">
+        <v>5</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>480</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>5</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>TRÜ, VKK 5, 58/62 (29)</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K41" t="n">
-        <v>5</v>
+          <t>["480D*"]</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_5_58_29.txt</t>
+        </is>
       </c>
       <c r="L41" t="inlineStr">
-        <is>
-          <t>["480D*"]</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_5_58_29.txt</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
         <is>
           <t xml:space="preserve">Жини-быки дед и зада
 у них ды догна дедова до
@@ -9033,13 +8475,6 @@
 </t>
         </is>
       </c>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -9067,37 +8502,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>9</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 9, 28/51 (3)</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K42" t="n">
-        <v>2</v>
+          <t>["300", "300A"]</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_9_28_3.txt</t>
+        </is>
       </c>
       <c r="L42" t="inlineStr">
-        <is>
-          <t>["300", "300A"]</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_9_28_3.txt</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
         <is>
           <t xml:space="preserve">был царь с царищей.
 жыли ани харашо, да вот
@@ -9532,13 +8963,6 @@
 </t>
         </is>
       </c>
-      <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
-      <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -9568,37 +8992,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>13</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 13, 23/6 (2)</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K43" t="n">
-        <v>2</v>
+          <t>["331", "1174", "1168"]</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_23_2.txt</t>
+        </is>
       </c>
       <c r="L43" t="inlineStr">
-        <is>
-          <t>["331", "1174", "1168"]</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_23_2.txt</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
         <is>
           <t xml:space="preserve">рес, никак
 ностанет Вышел - гаварит, - випе
@@ -9673,13 +9093,6 @@
 </t>
         </is>
       </c>
-      <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -9707,37 +9120,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F44" t="n">
+        <v>2</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>13</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 13, 31/46 (2)</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K44" t="n">
-        <v>2</v>
+          <t>["313"]</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_31_2.txt</t>
+        </is>
       </c>
       <c r="L44" t="inlineStr">
-        <is>
-          <t>["313"]</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_31_2.txt</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
         <is>
           <t xml:space="preserve">Шые цар с царицей.
 у них на была денейаг
@@ -10064,13 +9473,6 @@
 </t>
         </is>
       </c>
-      <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -10104,37 +9506,33 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F45" t="n">
+        <v>4</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>13</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 13, 59/80 (4)</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K45" t="n">
-        <v>4</v>
+          <t>["552", "302C*", "554", "556F*"]</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_59_4.txt</t>
+        </is>
       </c>
       <c r="L45" t="inlineStr">
-        <is>
-          <t>["552", "302C*", "554", "556F*"]</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>/Users/eugenia/Desktop/thesis/magic_tagger/data/processed/text_extraction/tru_vkk_13_59_4.txt</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
         <is>
           <t xml:space="preserve">неыя ноай-даревъ
 У няво было три
@@ -10616,13 +10014,6 @@
 </t>
         </is>
       </c>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -10650,37 +10041,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F46" t="n">
+        <v>5</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>480</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>48</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>TRÜ, VKK 48, 62/3 (110)</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K46" t="n">
-        <v>5</v>
-      </c>
-      <c r="L46" t="inlineStr"/>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr">
+          <t>["480D*"]</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr">
         <is>
           <t>от
  nar007
@@ -10732,27 +10115,6 @@
 блина не дам.</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P46" t="n">
-        <v>48</v>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 48, 62/3 (110)</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>480D*</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -10780,29 +10142,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>43</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 43, 8/10 (2)</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K47" t="n">
-        <v>2</v>
-      </c>
-      <c r="L47" t="inlineStr"/>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr">
+          <t>["425C"]</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr">
         <is>
           <t>nar001
  86 лет
@@ -10895,27 +10257,6 @@
  С.О.</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P47" t="n">
-        <v>43</v>
-      </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 43, 8/10 (2)</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>425C</t>
-        </is>
-      </c>
-      <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -10943,29 +10284,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F48" t="n">
+        <v>4</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>32</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 32, 14/6 (2)</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K48" t="n">
-        <v>4</v>
-      </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr">
+          <t>["552"]</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr">
         <is>
           <t>Записано от
  nar003.
@@ -11051,27 +10392,6 @@
  col015.</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P48" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 32, 14/6 (2)</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>552</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr"/>
-      <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -11099,29 +10419,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F49" t="n">
+        <v>3</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>32</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 32, 26/7 (5)</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K49" t="n">
-        <v>3</v>
-      </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="M49" t="inlineStr"/>
-      <c r="N49" t="inlineStr">
+          <t>["550"]</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr">
         <is>
           <t>Записано от
  nar004 (12
@@ -11167,27 +10487,6 @@
  col015.</t>
         </is>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P49" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 32, 26/7 (5)</t>
-        </is>
-      </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>550</t>
-        </is>
-      </c>
-      <c r="S49" t="inlineStr"/>
-      <c r="T49" t="inlineStr"/>
-      <c r="U49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -11218,37 +10517,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>SUS</t>
-        </is>
+      <c r="F50" t="n">
+        <v>6</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>707B*</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>mapped_from_local</t>
-        </is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>29</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>broad</t>
+          <t>TRÜ, VKK 29, 54/67 (68)</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K50" t="n">
-        <v>6</v>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr">
+          <t>["707"]</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr">
         <is>
           <t>В некатарам царстви, в некатарам
 государстви или в том, каторам мы
@@ -11555,27 +10846,6 @@
 около 60-ти лет</t>
         </is>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P50" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 29, 54/67 (68)</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>707</t>
-        </is>
-      </c>
-      <c r="S50" t="inlineStr"/>
-      <c r="T50" t="inlineStr"/>
-      <c r="U50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -11606,29 +10876,29 @@
           <t>v1_20251230</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>not_needed_native_atu</t>
-        </is>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>TRÜ, VKK</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>25</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>exact</t>
+          <t>TRÜ, VKK 25, 120/4 (23)</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>ok</t>
-        </is>
-      </c>
-      <c r="K51" t="n">
-        <v>1</v>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="M51" t="inlineStr"/>
-      <c r="N51" t="inlineStr">
+          <t>["327A", "707"]</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr">
         <is>
           <t>Была вбатки три
 дацке Была уних наронаjа
@@ -11741,31 +11011,6 @@
 эта моj папаша. Ифсо.</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK</t>
-        </is>
-      </c>
-      <c r="P51" t="n">
-        <v>25</v>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>TRÜ, VKK 25, 120/4 (23)</t>
-        </is>
-      </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>327A</t>
-        </is>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>707</t>
-        </is>
-      </c>
-      <c r="T51" t="inlineStr"/>
-      <c r="U51" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>